<commit_message>
Documentos 3 puntos apache
</commit_message>
<xml_diff>
--- a/BoletinEjercicios.xlsx
+++ b/BoletinEjercicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\GitHub\Master\Master_ADSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE01A93-8373-474B-9459-013A89187BA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A110330-5035-4A22-833D-3360BF8EC2CE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{A6F86383-F6B4-477E-A0CE-71D844BC3BAB}"/>
   </bookViews>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="B4" s="66">
         <f>'Apache (Politicas)'!F1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="B10" s="99">
         <f>SUM(B3:B9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4411,8 +4411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DF5160-4284-4FEF-A742-DD5BF6903890}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4434,14 +4434,14 @@
       </c>
       <c r="D1" s="68">
         <f>E6+E12+E24+E34</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="69" t="s">
         <v>542</v>
       </c>
       <c r="F1" s="68">
         <f>D1+D2</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="E12" s="51">
         <f>SUMPRODUCT($C13:$C23,E13:E23)</f>
-        <v>0.60000000000000009</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="13" spans="1:6" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4640,7 +4640,9 @@
         <v>0.2</v>
       </c>
       <c r="D16" s="72"/>
-      <c r="E16" s="70"/>
+      <c r="E16" s="70">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="51" t="s">
@@ -4653,7 +4655,9 @@
         <v>0.2</v>
       </c>
       <c r="D17" s="72"/>
-      <c r="E17" s="70"/>
+      <c r="E17" s="70">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
@@ -4666,7 +4670,9 @@
         <v>0.2</v>
       </c>
       <c r="D18" s="72"/>
-      <c r="E18" s="70"/>
+      <c r="E18" s="70">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:5" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="51" t="s">
@@ -4718,7 +4724,9 @@
         <v>0.4</v>
       </c>
       <c r="D22" s="72"/>
-      <c r="E22" s="70"/>
+      <c r="E22" s="70">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:5" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="51" t="s">

</xml_diff>